<commit_message>
test app update 20221214
</commit_message>
<xml_diff>
--- a/Log/testcase_log_result.xlsx
+++ b/Log/testcase_log_result.xlsx
@@ -571,7 +571,7 @@
       </c>
       <c r="F2" s="13" t="inlineStr">
         <is>
-          <t>17:27:46 2022/11/22</t>
+          <t>16:37:16 2022/12/14</t>
         </is>
       </c>
       <c r="G2" s="13" t="inlineStr">
@@ -581,7 +581,7 @@
       </c>
       <c r="I2" s="14" t="inlineStr">
         <is>
-          <t>221122172807</t>
+          <t>221214165117</t>
         </is>
       </c>
       <c r="J2" s="14" t="inlineStr"/>
@@ -619,7 +619,7 @@
       </c>
       <c r="F3" s="13" t="inlineStr">
         <is>
-          <t>17:27:46 2022/11/22</t>
+          <t>16:37:16 2022/12/14</t>
         </is>
       </c>
       <c r="G3" s="13" t="inlineStr">
@@ -656,7 +656,7 @@
       </c>
       <c r="F4" s="13" t="inlineStr">
         <is>
-          <t>17:27:46 2022/11/22</t>
+          <t>16:37:16 2022/12/14</t>
         </is>
       </c>
       <c r="G4" s="13" t="inlineStr">
@@ -693,7 +693,7 @@
       </c>
       <c r="F5" s="13" t="inlineStr">
         <is>
-          <t>17:27:46 2022/11/22</t>
+          <t>16:37:16 2022/12/14</t>
         </is>
       </c>
       <c r="G5" s="13" t="inlineStr">

</xml_diff>